<commit_message>
vault backup: 2025-04-14 11:50:54
</commit_message>
<xml_diff>
--- a/2 - РАбОТА/Списание/Счета/Для списания ЗИП номера счетов Сибирский банк (1).xlsx
+++ b/2 - РАбОТА/Списание/Счета/Для списания ЗИП номера счетов Сибирский банк (1).xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esitnikov\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OBSIDIAN\DisparuDEP\2 - РАбОТА\Списание\Счета\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6466EB7E-DC0D-4585-9FFA-B4F9AAC70B41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="-120" windowWidth="38640" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23880" yWindow="-120" windowWidth="38640" windowHeight="15990"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$A$1:$D$41</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="132">
   <si>
     <t>Дата</t>
   </si>
@@ -391,12 +390,45 @@
   </si>
   <si>
     <t xml:space="preserve">декабрь 2024г. </t>
+  </si>
+  <si>
+    <t>ТДР00000275 от 16.04.2021</t>
+  </si>
+  <si>
+    <t>ТДР00000329 от 11.05.2021</t>
+  </si>
+  <si>
+    <t>ТДР00000641 от 10.08.2021</t>
+  </si>
+  <si>
+    <t>ТДР00000464 от 13.07.2021</t>
+  </si>
+  <si>
+    <t>ТДР00000384 от 15.06.2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ТДР00000766 от 07.10.2021</t>
+  </si>
+  <si>
+    <t>ТДР00000667 от 31.08.2021</t>
+  </si>
+  <si>
+    <t>ТДР00000872 от 23.11.2021</t>
+  </si>
+  <si>
+    <t>ТДР00000959 от 15.12.2021</t>
+  </si>
+  <si>
+    <t>ТДР00000015 от 14.01.2022</t>
+  </si>
+  <si>
+    <t>ТДР00000766 от 07.10.2021</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -490,7 +522,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Обычный_Лист1" xfId="1" xr:uid="{D03757F1-F8A2-4D62-978B-C5AFA1B5744A}"/>
+    <cellStyle name="Обычный_Лист1" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -767,10 +799,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -780,7 +814,7 @@
     <col min="4" max="4" width="57.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -794,7 +828,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -808,7 +842,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -822,7 +856,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -835,8 +869,11 @@
       <c r="D4" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -849,8 +886,11 @@
       <c r="D5" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -863,8 +903,11 @@
       <c r="D6" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -877,8 +920,11 @@
       <c r="D7" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
@@ -891,8 +937,14 @@
       <c r="D8" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>123</v>
+      </c>
+      <c r="H8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
@@ -905,8 +957,11 @@
       <c r="D9" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
@@ -919,8 +974,11 @@
       <c r="D10" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
@@ -933,8 +991,14 @@
       <c r="D11" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>128</v>
+      </c>
+      <c r="H11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
@@ -947,8 +1011,11 @@
       <c r="D12" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>28</v>
       </c>
@@ -961,8 +1028,11 @@
       <c r="D13" s="1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>29</v>
       </c>
@@ -976,7 +1046,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>31</v>
       </c>
@@ -990,7 +1060,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>33</v>
       </c>
@@ -1355,7 +1425,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D41" xr:uid="{A24C6A1C-8CEA-4BD7-A12B-74925A997BF7}"/>
+  <autoFilter ref="A1:D41"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>